<commit_message>
Implementacion de Persona y lista paginadas
</commit_message>
<xml_diff>
--- a/ScriptInstalacion/05_SistemaInformacionInicial.xlsx
+++ b/ScriptInstalacion/05_SistemaInformacionInicial.xlsx
@@ -9,20 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="23715" windowHeight="9525" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="23715" windowHeight="9525" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="01_CATALOGO" sheetId="1" r:id="rId1"/>
     <sheet name="02_ITEM_CATALOGO" sheetId="2" r:id="rId2"/>
     <sheet name="03_MODULOS" sheetId="3" r:id="rId3"/>
     <sheet name="04_MODULOS_FUNCIONALIDADES" sheetId="4" r:id="rId4"/>
+    <sheet name="Hoja1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="125">
   <si>
     <t>CODIGO</t>
   </si>
@@ -382,6 +383,21 @@
   </si>
   <si>
     <t>PARAMETRIZACIONES</t>
+  </si>
+  <si>
+    <t>NAMESPACE</t>
+  </si>
+  <si>
+    <t>PersonaNatural</t>
+  </si>
+  <si>
+    <t>JusNucleo.Bl.Personas</t>
+  </si>
+  <si>
+    <t>FUCIONALIDAD_CODIGO</t>
+  </si>
+  <si>
+    <t>/Index</t>
   </si>
 </sst>
 </file>
@@ -1551,7 +1567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1628,8 +1644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1637,8 +1653,8 @@
     <col min="1" max="1" width="24.5703125" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" customWidth="1"/>
-    <col min="5" max="5" width="5" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1"/>
     <col min="6" max="6" width="9.85546875" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.5703125" customWidth="1"/>
@@ -1739,7 +1755,10 @@
         <v>111</v>
       </c>
       <c r="D4" t="s">
-        <v>105</v>
+        <v>121</v>
+      </c>
+      <c r="E4" t="s">
+        <v>124</v>
       </c>
       <c r="G4" t="s">
         <v>5</v>
@@ -1752,7 +1771,7 @@
       </c>
       <c r="J4" t="str">
         <f>CONCATENATE("call PRC_INS_FUNCIONALIDADES('",I4,"','",VLOOKUP(I4,'03_MODULOS'!A:D,2,FALSE),"','",VLOOKUP(I4,'03_MODULOS'!A:D,3,FALSE),"','",VLOOKUP(I4,'03_MODULOS'!A:D,4,FALSE),"','",A4,"','",B4,"','",,C4,"','",D4,"','",E4,"','",F4,"','",G4,"','",H4,"','",I4,"');")</f>
-        <v>call PRC_INS_FUNCIONALIDADES('MODREGIS','REGISTRO','REGISTRO','SIS001','FUNPERSONA','PERSONAS','PERSONAS','/','','','ACTIVO','I,O,A,B','MODREGIS');</v>
+        <v>call PRC_INS_FUNCIONALIDADES('MODREGIS','REGISTRO','REGISTRO','SIS001','FUNPERSONA','PERSONAS','PERSONAS','PersonaNatural','/Index','','ACTIVO','I,O,A,B','MODREGIS');</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1780,6 +1799,48 @@
       <c r="J5" t="str">
         <f>CONCATENATE("call PRC_INS_FUNCIONALIDADES('",I5,"','",VLOOKUP(I5,'03_MODULOS'!A:D,2,FALSE),"','",VLOOKUP(I5,'03_MODULOS'!A:D,3,FALSE),"','",VLOOKUP(I5,'03_MODULOS'!A:D,4,FALSE),"','",A5,"','",B5,"','",,C5,"','",D5,"','",E5,"','",F5,"','",G5,"','",H5,"','",I5,"');")</f>
         <v>call PRC_INS_FUNCIONALIDADES('MODCONFIG','CONFIGURACIÓN','CONFIGURACIÓN','SIS001','FUNPARAME','PARMETRIZACIONES','PARAMETRIZACIONES','/','','','ACTIVO','I,O,A,B','MODCONFIG');</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>